<commit_message>
add flipcards for phrases (now works on firefox too)
</commit_message>
<xml_diff>
--- a/Data/phrases.xlsx
+++ b/Data/phrases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitken/Documents/Personal/Chinese/Zhongwen/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B48A67-5597-704B-B384-3C8C15363A10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C83CEA3-EA19-584A-9EBD-4FBD24A78CD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{790C4370-7197-2047-A56B-DE58D82A558A}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>Nǐ jiào shénme míngzi?</t>
   </si>
   <si>
-    <t>你叫什么名字？</t>
+    <t>你叫什么名字?</t>
   </si>
 </sst>
 </file>
@@ -460,13 +460,14 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="211" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix lesson select code, card widths + card creation
</commit_message>
<xml_diff>
--- a/Data/phrases.xlsx
+++ b/Data/phrases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitken/Documents/Personal/Chinese/Zhongwen/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C83CEA3-EA19-584A-9EBD-4FBD24A78CD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B91A814-6BE9-1545-8E02-3FD4B4F12659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{790C4370-7197-2047-A56B-DE58D82A558A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>english</t>
   </si>
@@ -105,7 +105,25 @@
     <t>Nǐ jiào shénme míngzi?</t>
   </si>
   <si>
-    <t>你叫什么名字?</t>
+    <t>你叫什么名字？</t>
+  </si>
+  <si>
+    <t>Rènshi nǐ hěn gāoxing</t>
+  </si>
+  <si>
+    <t>认识你很高兴</t>
+  </si>
+  <si>
+    <t>Glad to meet you</t>
+  </si>
+  <si>
+    <t>Can I give you a call?</t>
+  </si>
+  <si>
+    <t>Kěyǐ gěi nǐ dǎ diànhuà ma?</t>
+  </si>
+  <si>
+    <t>可以你打电话吗？</t>
   </si>
 </sst>
 </file>
@@ -457,17 +475,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60032F5C-C47F-4F4D-82AB-0D1A2BBCFB1D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="211" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -582,6 +600,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update phrases and vocab with lesson 4 content
</commit_message>
<xml_diff>
--- a/Data/phrases.xlsx
+++ b/Data/phrases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitken/Documents/Personal/Chinese/Zhongwen/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B91A814-6BE9-1545-8E02-3FD4B4F12659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B83C564-05DF-4D42-9008-7C991351AA68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{790C4370-7197-2047-A56B-DE58D82A558A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>english</t>
   </si>
@@ -99,9 +99,6 @@
     <t>再见</t>
   </si>
   <si>
-    <t>What's your name?</t>
-  </si>
-  <si>
     <t>Nǐ jiào shénme míngzi?</t>
   </si>
   <si>
@@ -124,6 +121,180 @@
   </si>
   <si>
     <t>可以你打电话吗？</t>
+  </si>
+  <si>
+    <t>This map is in English</t>
+  </si>
+  <si>
+    <t>Zhè zhāng dìtú shì yīngwén de</t>
+  </si>
+  <si>
+    <t>这张地图是英文的</t>
+  </si>
+  <si>
+    <t>你有没有中国地图?</t>
+  </si>
+  <si>
+    <t>Do you have a map of China?</t>
+  </si>
+  <si>
+    <t>Nǐ yǒu méiyǒu Zhōngguó dìtú?</t>
+  </si>
+  <si>
+    <t>I'll have a look</t>
+  </si>
+  <si>
+    <t>Wǒ kàn yíxià</t>
+  </si>
+  <si>
+    <t>我看一下</t>
+  </si>
+  <si>
+    <t>Why do you want to look at a map of China?</t>
+  </si>
+  <si>
+    <t>Nǐ kàn Zhōngguó dìtú gàn shénme?</t>
+  </si>
+  <si>
+    <t>I know</t>
+  </si>
+  <si>
+    <t>Wǒ zhīdao</t>
+  </si>
+  <si>
+    <t>我知道</t>
+  </si>
+  <si>
+    <t>I want a book</t>
+  </si>
+  <si>
+    <t>Wǒ yào yì běn shū</t>
+  </si>
+  <si>
+    <t>我要一本书</t>
+  </si>
+  <si>
+    <t>What are you doing?</t>
+  </si>
+  <si>
+    <t>Do you know Mandarin?</t>
+  </si>
+  <si>
+    <t>Nǐ zhīdào hànyǔ ma?</t>
+  </si>
+  <si>
+    <t>Nǐ zài gàn shénme?</t>
+  </si>
+  <si>
+    <t>你在干什么？</t>
+  </si>
+  <si>
+    <t>你知道汉语吗？</t>
+  </si>
+  <si>
+    <t>你看中国地图干什么？</t>
+  </si>
+  <si>
+    <t>What is your nationality?</t>
+  </si>
+  <si>
+    <t>Nǐ shì nǎ guó rén?</t>
+  </si>
+  <si>
+    <t>你是哪国人？</t>
+  </si>
+  <si>
+    <t>Duìbuqǐ, wǒ bù zhīdào</t>
+  </si>
+  <si>
+    <t>去不起, 我不知道</t>
+  </si>
+  <si>
+    <t>What is your name?</t>
+  </si>
+  <si>
+    <t>My home is relatively small</t>
+  </si>
+  <si>
+    <t>Wǒ jiā bǐjiào xiǎo</t>
+  </si>
+  <si>
+    <t>我家比较小</t>
+  </si>
+  <si>
+    <t>那个电影真有意思</t>
+  </si>
+  <si>
+    <t>This book is very useful</t>
+  </si>
+  <si>
+    <t>Sorry, I do not know</t>
+  </si>
+  <si>
+    <t>Do you like reading books?</t>
+  </si>
+  <si>
+    <t>Nǐ xǐhuān kànshū ma?</t>
+  </si>
+  <si>
+    <t>你喜欢看书吗？</t>
+  </si>
+  <si>
+    <t>Excuse me, may I have a pen?</t>
+  </si>
+  <si>
+    <t>Qǐngwèn, wǒ kěyǐ yào yī zhī bǐ ma?</t>
+  </si>
+  <si>
+    <t>请问，我可以要一支笔吗？</t>
+  </si>
+  <si>
+    <t>Whose book is this?</t>
+  </si>
+  <si>
+    <t>Can I look at your map?</t>
+  </si>
+  <si>
+    <t>这本书是谁的？</t>
+  </si>
+  <si>
+    <t>Wǒ néng kàn yíxià nǐ de dìtú ma</t>
+  </si>
+  <si>
+    <t>我能看一下你的地图吗？</t>
+  </si>
+  <si>
+    <t>Zhè běn shū shì shéide?</t>
+  </si>
+  <si>
+    <t>Of course, you can use my notebook</t>
+  </si>
+  <si>
+    <t>Dāngrán, nǐ kěyǐ yòng wǒ de běnzi</t>
+  </si>
+  <si>
+    <t>当然, 你可以用我的本子</t>
+  </si>
+  <si>
+    <t>Can I ask a question?</t>
+  </si>
+  <si>
+    <t>Wǒ néng wèn yígè wèntí ma?</t>
+  </si>
+  <si>
+    <t>我能问一个问题吗？</t>
+  </si>
+  <si>
+    <t>这本书非常有用</t>
+  </si>
+  <si>
+    <t>That movie is really interesting</t>
+  </si>
+  <si>
+    <t>Nàgè diànyǐng zhēn yǒu yìsi</t>
+  </si>
+  <si>
+    <t>Zhè běn shū fēicháng yǒu yòng</t>
   </si>
 </sst>
 </file>
@@ -475,17 +646,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60032F5C-C47F-4F4D-82AB-0D1A2BBCFB1D}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="211" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -588,13 +759,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -602,30 +773,296 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>